<commit_message>
User sign inand User change password test cases added
</commit_message>
<xml_diff>
--- a/MVPStudioAdvancedSprint/LoginCred.xlsx
+++ b/MVPStudioAdvancedSprint/LoginCred.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raj4s\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MVPStudioAdvacedSprint\MVPStudioAdvancedSprint\MVPStudioAdvancedSprint\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3DB0C4AC-A86D-46D1-8DFA-30C54CF8D776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855B2ADC-1CD1-4003-9258-102E7D9D0A28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{A00620A7-6FB2-4538-AF45-CD491D229E33}"/>
+    <workbookView xWindow="3915" yWindow="840" windowWidth="21600" windowHeight="11055" xr2:uid="{A00620A7-6FB2-4538-AF45-CD491D229E33}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Username</t>
   </si>
@@ -46,6 +46,24 @@
   </si>
   <si>
     <t>IndustryConnect2023</t>
+  </si>
+  <si>
+    <t>GOWgow@GOW.com</t>
+  </si>
+  <si>
+    <t>santamonica</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>LastOfUs@LOS.com</t>
+  </si>
+  <si>
+    <t>naughtydog</t>
+  </si>
+  <si>
+    <t>LastofUS@los.com</t>
   </si>
 </sst>
 </file>
@@ -400,7 +418,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -408,37 +426,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{098140FE-8508-4923-AB99-3B41AC872C59}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{2B17A1AD-081A-476E-842C-B3FF77224F61}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{6E519386-2555-4852-B4EF-23F45CB7AA5B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Extent report file path updated
</commit_message>
<xml_diff>
--- a/MVPStudioAdvancedSprint/LoginCred.xlsx
+++ b/MVPStudioAdvancedSprint/LoginCred.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MVPStudioAdvacedSprint\MVPStudioAdvancedSprint\MVPStudioAdvancedSprint\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855B2ADC-1CD1-4003-9258-102E7D9D0A28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BACF26C-6CEC-4EF5-9272-DF166D883B5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3915" yWindow="840" windowWidth="21600" windowHeight="11055" xr2:uid="{A00620A7-6FB2-4538-AF45-CD491D229E33}"/>
+    <workbookView xWindow="3480" yWindow="1995" windowWidth="21600" windowHeight="11055" xr2:uid="{A00620A7-6FB2-4538-AF45-CD491D229E33}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Username</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>LastofUS@los.com</t>
+  </si>
+  <si>
+    <t>LastOFUs@LOS.com</t>
+  </si>
+  <si>
+    <t>LaStofUS@los.com</t>
   </si>
 </sst>
 </file>
@@ -426,7 +432,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{098140FE-8508-4923-AB99-3B41AC872C59}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:XFD4"/>
@@ -493,6 +499,28 @@
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{2B17A1AD-081A-476E-842C-B3FF77224F61}"/>

</xml_diff>

<commit_message>
MVP advanced sprint add tests --> user description-->refine code
</commit_message>
<xml_diff>
--- a/MVPStudioAdvancedSprint/LoginCred.xlsx
+++ b/MVPStudioAdvancedSprint/LoginCred.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MVPStudioAdvacedSprint\MVPStudioAdvancedSprint\MVPStudioAdvancedSprint\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BACF26C-6CEC-4EF5-9272-DF166D883B5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{441141B3-9D23-47AF-A107-012E40E2EAC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="1995" windowWidth="21600" windowHeight="11055" xr2:uid="{A00620A7-6FB2-4538-AF45-CD491D229E33}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A00620A7-6FB2-4538-AF45-CD491D229E33}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
   <si>
     <t>Username</t>
   </si>
@@ -42,18 +42,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>raj4shr@gmail.com</t>
-  </si>
-  <si>
-    <t>IndustryConnect2023</t>
-  </si>
-  <si>
-    <t>GOWgow@GOW.com</t>
-  </si>
-  <si>
-    <t>santamonica</t>
-  </si>
-  <si>
     <t>Id</t>
   </si>
   <si>
@@ -70,24 +58,31 @@
   </si>
   <si>
     <t>LaStofUS@los.com</t>
+  </si>
+  <si>
+    <t>LAstOFUs@LOS.com</t>
+  </si>
+  <si>
+    <t>LAStofUS@los.com</t>
+  </si>
+  <si>
+    <t>GOWgow@GOW.com.com.com</t>
+  </si>
+  <si>
+    <t>santa monica</t>
+  </si>
+  <si>
+    <t>LAStOFUs@LOS.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -110,16 +105,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -432,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{098140FE-8508-4923-AB99-3B41AC872C59}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,26 +444,26 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
+      <c r="A2" t="s">
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
+      <c r="A3" t="s">
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -479,10 +471,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -490,10 +482,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -501,10 +493,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -512,20 +504,49 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{2B17A1AD-081A-476E-842C-B3FF77224F61}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{6E519386-2555-4852-B4EF-23F45CB7AA5B}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>